<commit_message>
Added USA data exculding trade
</commit_message>
<xml_diff>
--- a/dataSources/Regionalization.xlsx
+++ b/dataSources/Regionalization.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\trevorb\repositories\Canada-U.S.-ElecTrade\dataSources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F20166-E1CA-489F-A67B-72D66E38ADB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5BB1223-B990-4CDC-A280-A36B521A6907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="0" windowWidth="16920" windowHeight="10540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33720" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CAN" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>REGION</t>
   </si>
@@ -69,6 +69,42 @@
   </si>
   <si>
     <t>AT</t>
+  </si>
+  <si>
+    <t>NW</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>MN</t>
+  </si>
+  <si>
+    <t>SW</t>
+  </si>
+  <si>
+    <t>CE</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>NE</t>
   </si>
 </sst>
 </file>
@@ -911,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1012,12 +1048,85 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>